<commit_message>
refactor after strucutre change
</commit_message>
<xml_diff>
--- a/GUI.xlsx
+++ b/GUI.xlsx
@@ -1,23 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\GitHub\Energy-Balance-Model\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C120AE83-7165-4036-B537-D0B87E83A882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="storage_data"/>
-    <sheet r:id="rId2" sheetId="2" name="pvt_data"/>
-    <sheet r:id="rId3" sheetId="3" name="house_data"/>
-    <sheet r:id="rId4" sheetId="4" name="mediator_data"/>
+    <sheet name="storage_data" sheetId="1" r:id="rId1"/>
+    <sheet name="pvt_data" sheetId="2" r:id="rId2"/>
+    <sheet name="house_data" sheetId="3" r:id="rId3"/>
+    <sheet name="mediator_data" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>storage_is_included</t>
   </si>
@@ -143,12 +159,15 @@
   </si>
   <si>
     <t>init_charging_temp</t>
+  </si>
+  <si>
+    <t>tim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
@@ -195,50 +214,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -249,10 +268,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -290,71 +309,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -382,7 +401,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -405,11 +424,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -418,13 +437,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -434,7 +453,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -443,7 +462,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -452,7 +471,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -460,10 +479,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -528,34 +547,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="8.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="33.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="4" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="5" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -598,9 +618,11 @@
       <c r="N1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="1"/>
+      <c r="O1" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+    <row r="2" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -644,6 +666,11 @@
         <v>50</v>
       </c>
       <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -651,7 +678,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -661,28 +688,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="9.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="22.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="22.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="21.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="5" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="5" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="5" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="5" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="8" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -741,7 +767,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -758,10 +784,10 @@
         <v>3.37</v>
       </c>
       <c r="F2" s="6">
-        <v>0.0104</v>
+        <v>1.04E-2</v>
       </c>
       <c r="G2" s="10">
-        <v>0.0125</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="H2" s="2">
         <v>3600</v>
@@ -806,26 +832,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -848,7 +874,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -877,7 +903,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -887,17 +913,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="3" width="19" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -923,15 +947,18 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
-      <c r="A2" s="3">
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="str">
         <f>storage_data!A2</f>
-      </c>
-      <c r="B2" s="3">
+        <v>true</v>
+      </c>
+      <c r="B2" s="3" t="str">
         <f>pvt_data!A2</f>
-      </c>
-      <c r="C2" s="3">
+        <v>true</v>
+      </c>
+      <c r="C2" s="3" t="str">
         <f>house_data!A2</f>
+        <v>true</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
checked energy balance and autarky issues
</commit_message>
<xml_diff>
--- a/GUI.xlsx
+++ b/GUI.xlsx
@@ -1,39 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\GitHub\Energy-Balance-Model\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C120AE83-7165-4036-B537-D0B87E83A882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="storage_data" sheetId="1" r:id="rId1"/>
-    <sheet name="pvt_data" sheetId="2" r:id="rId2"/>
-    <sheet name="house_data" sheetId="3" r:id="rId3"/>
-    <sheet name="mediator_data" sheetId="4" r:id="rId4"/>
+    <sheet r:id="rId1" sheetId="1" name="storage_data"/>
+    <sheet r:id="rId2" sheetId="2" name="pvt_data"/>
+    <sheet r:id="rId3" sheetId="3" name="house_data"/>
+    <sheet r:id="rId4" sheetId="4" name="mediator_data"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>storage_is_included</t>
   </si>
@@ -161,13 +145,13 @@
     <t>init_charging_temp</t>
   </si>
   <si>
-    <t>tim</t>
+    <t>false</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
@@ -215,49 +199,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -268,10 +255,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -309,71 +296,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -401,7 +388,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -424,11 +411,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -437,13 +424,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -453,7 +440,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -462,7 +449,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -471,7 +458,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -479,10 +466,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -547,35 +534,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="8.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="5" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="26.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="5" width="33.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="4" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="5" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -618,11 +604,9 @@
       <c r="N1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="12" t="s">
-        <v>42</v>
-      </c>
+      <c r="O1" s="12"/>
     </row>
-    <row r="2" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -660,17 +644,29 @@
         <v>10</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="N2" s="2">
         <v>50</v>
       </c>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>42</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -678,7 +674,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -688,27 +684,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="9.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="22.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="22.005" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="5" width="21.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="5" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="5" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="5" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="5" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="8" width="12.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -767,7 +764,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -784,10 +781,10 @@
         <v>3.37</v>
       </c>
       <c r="F2" s="6">
-        <v>1.04E-2</v>
+        <v>0.0104</v>
       </c>
       <c r="G2" s="10">
-        <v>1.2500000000000001E-2</v>
+        <v>0.0125</v>
       </c>
       <c r="H2" s="2">
         <v>3600</v>
@@ -832,26 +829,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="15.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -874,7 +871,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -894,7 +891,7 @@
         <v>25</v>
       </c>
       <c r="G2" s="7">
-        <v>0.2</v>
+        <v>0.225</v>
       </c>
     </row>
   </sheetData>
@@ -903,7 +900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -913,15 +910,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="19" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="24.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -947,18 +946,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="str">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+      <c r="A2" s="3">
         <f>storage_data!A2</f>
-        <v>true</v>
-      </c>
-      <c r="B2" s="3" t="str">
+      </c>
+      <c r="B2" s="3">
         <f>pvt_data!A2</f>
-        <v>true</v>
-      </c>
-      <c r="C2" s="3" t="str">
+      </c>
+      <c r="C2" s="3">
         <f>house_data!A2</f>
-        <v>true</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
fixed energy balance and added repetition period
</commit_message>
<xml_diff>
--- a/GUI.xlsx
+++ b/GUI.xlsx
@@ -1,18 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\GitHub\Energy-Balance-Model\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1B5FFD-E0DA-4C6E-BA94-A265BF6FEA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="storage_data"/>
-    <sheet r:id="rId2" sheetId="2" name="pvt_data"/>
-    <sheet r:id="rId3" sheetId="3" name="house_data"/>
-    <sheet r:id="rId4" sheetId="4" name="mediator_data"/>
+    <sheet name="storage_data" sheetId="1" r:id="rId1"/>
+    <sheet name="pvt_data" sheetId="2" r:id="rId2"/>
+    <sheet name="house_data" sheetId="3" r:id="rId3"/>
+    <sheet name="mediator_data" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -145,13 +161,13 @@
     <t>init_charging_temp</t>
   </si>
   <si>
-    <t>false</t>
+    <t>repetition_period</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
@@ -199,52 +215,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -255,10 +268,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -296,71 +309,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -388,7 +401,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -411,11 +424,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -424,13 +437,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -440,7 +453,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -449,7 +462,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -458,7 +471,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -466,10 +479,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -534,34 +547,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="8.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="33.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="4" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="5" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -606,7 +620,7 @@
       </c>
       <c r="O1" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+    <row r="2" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -643,15 +657,15 @@
       <c r="L2" s="2">
         <v>10</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>42</v>
+      <c r="M2" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="N2" s="2">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="O2" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+    <row r="3" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -674,7 +688,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -684,28 +698,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="9.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="22.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="22.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="21.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="5" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="5" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="5" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="5" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="8" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -764,7 +777,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -781,10 +794,10 @@
         <v>3.37</v>
       </c>
       <c r="F2" s="6">
-        <v>0.0104</v>
+        <v>1.04E-2</v>
       </c>
       <c r="G2" s="10">
-        <v>0.0125</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="H2" s="2">
         <v>3600</v>
@@ -829,26 +842,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -871,7 +886,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -891,7 +906,7 @@
         <v>25</v>
       </c>
       <c r="G2" s="7">
-        <v>0.225</v>
+        <v>0.16</v>
       </c>
     </row>
   </sheetData>
@@ -900,27 +915,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="3" width="19" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -945,16 +961,22 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
-      <c r="A2" s="3">
+    <row r="2" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="str">
         <f>storage_data!A2</f>
-      </c>
-      <c r="B2" s="3">
+        <v>true</v>
+      </c>
+      <c r="B2" s="3" t="str">
         <f>pvt_data!A2</f>
-      </c>
-      <c r="C2" s="3">
+        <v>true</v>
+      </c>
+      <c r="C2" s="3" t="str">
         <f>house_data!A2</f>
+        <v>true</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -970,6 +992,9 @@
       </c>
       <c r="H2" s="2">
         <v>3600</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added HP and PV, working with layers
</commit_message>
<xml_diff>
--- a/GUI.xlsx
+++ b/GUI.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\GitHub\Energy-Balance-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1B5FFD-E0DA-4C6E-BA94-A265BF6FEA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC41FAF-6FB7-485A-B039-6F5B01FC5C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="storage_data" sheetId="1" r:id="rId1"/>
     <sheet name="pvt_data" sheetId="2" r:id="rId2"/>
     <sheet name="house_data" sheetId="3" r:id="rId3"/>
-    <sheet name="mediator_data" sheetId="4" r:id="rId4"/>
+    <sheet name="hp_data" sheetId="6" r:id="rId4"/>
+    <sheet name="pv_data" sheetId="7" r:id="rId5"/>
+    <sheet name="weather_data" sheetId="8" r:id="rId6"/>
+    <sheet name="mediator_data" sheetId="4" r:id="rId7"/>
+    <sheet name="simulator_data" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>storage_is_included</t>
   </si>
@@ -59,18 +63,9 @@
     <t>time_step</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>Luzern</t>
   </si>
   <si>
-    <t>TRUE</t>
-  </si>
-  <si>
-    <t>is_included</t>
-  </si>
-  <si>
     <t>heating_demand</t>
   </si>
   <si>
@@ -125,9 +120,6 @@
     <t>collector_temp</t>
   </si>
   <si>
-    <t>solar_latitute</t>
-  </si>
-  <si>
     <t>tank_height</t>
   </si>
   <si>
@@ -162,6 +154,39 @@
   </si>
   <si>
     <t>repetition_period</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>cell_efficiency</t>
+  </si>
+  <si>
+    <t>second_law_efficiency</t>
+  </si>
+  <si>
+    <t>is_air_source</t>
+  </si>
+  <si>
+    <t>solar_latitude</t>
+  </si>
+  <si>
+    <t>pv_is_included</t>
+  </si>
+  <si>
+    <t>connection_pv_hp</t>
+  </si>
+  <si>
+    <t>hp_charges_storage</t>
+  </si>
+  <si>
+    <t>hp_is_included</t>
+  </si>
+  <si>
+    <t>storage_charging_strategy</t>
+  </si>
+  <si>
+    <t>equally distributed</t>
   </si>
 </sst>
 </file>
@@ -551,136 +576,112 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
+    <row r="1" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="L1" s="12"/>
+    </row>
+    <row r="2" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
         <v>40</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" s="12"/>
-    </row>
-    <row r="2" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2</v>
-      </c>
       <c r="C2" s="2">
-        <v>40</v>
-      </c>
-      <c r="D2" s="2">
         <v>10</v>
       </c>
-      <c r="E2" s="2">
-        <v>3600</v>
+      <c r="D2" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.02</v>
       </c>
       <c r="F2" s="2">
-        <v>8760</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="H2" s="6">
         <v>0.02</v>
       </c>
+      <c r="G2" s="2">
+        <v>95</v>
+      </c>
+      <c r="H2" s="2">
+        <v>20</v>
+      </c>
       <c r="I2" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="J2" s="2">
-        <v>95</v>
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="K2" s="2">
-        <v>20</v>
-      </c>
-      <c r="L2" s="2">
-        <v>10</v>
-      </c>
-      <c r="M2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="N2" s="2">
         <v>35</v>
       </c>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="J3" s="1"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="1"/>
+      <c r="L3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -692,148 +693,108 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="6" t="s">
+    <row r="1" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>15</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="B2" s="6">
+        <v>3.37</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1.04E-2</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="E2" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2">
-        <v>3600</v>
-      </c>
-      <c r="C2" s="2">
-        <v>8760</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0.75</v>
-      </c>
-      <c r="E2" s="6">
-        <v>3.37</v>
-      </c>
-      <c r="F2" s="6">
-        <v>1.04E-2</v>
-      </c>
-      <c r="G2" s="10">
-        <v>1.2500000000000001E-2</v>
+      <c r="F2" s="2">
+        <v>90</v>
+      </c>
+      <c r="G2" s="2">
+        <v>30</v>
       </c>
       <c r="H2" s="2">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="I2" s="2">
-        <v>8760</v>
+        <v>160</v>
       </c>
       <c r="J2" s="2">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K2" s="2">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="L2" s="2">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2">
-        <v>160</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>95</v>
-      </c>
-      <c r="R2" s="2">
         <v>14</v>
-      </c>
-      <c r="S2" s="6">
-        <v>46.6</v>
       </c>
     </row>
   </sheetData>
@@ -846,7 +807,111 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>115</v>
+      </c>
+      <c r="B2" s="2">
+        <v>900</v>
+      </c>
+      <c r="C2" s="2">
+        <v>14</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>25</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0.16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61341AFE-9F70-4FA7-8BF0-845A144E344F}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11000</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB94CDB9-61E1-4932-B3E2-8E1E2BED6CDC}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
@@ -854,59 +919,108 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
+    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>0.23</v>
+      </c>
+      <c r="B2" s="2">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2">
+        <v>90</v>
+      </c>
+      <c r="D2" s="2">
+        <v>30</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>160</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
         <v>14</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D84336-4BDD-4290-B4B8-8FB7312C2A0E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2">
-        <v>115</v>
-      </c>
-      <c r="C2" s="2">
-        <v>900</v>
-      </c>
-      <c r="D2" s="2">
-        <v>14</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="F2" s="2">
-        <v>25</v>
-      </c>
-      <c r="G2" s="7">
-        <v>0.16</v>
+      <c r="B2">
+        <v>46.6</v>
       </c>
     </row>
   </sheetData>
@@ -914,29 +1028,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="19" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19" style="4" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -946,54 +1062,108 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C781A6E-1115-4E08-A78E-093D8B9DB9B9}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="str">
-        <f>storage_data!A2</f>
-        <v>true</v>
-      </c>
-      <c r="B2" s="3" t="str">
-        <f>pvt_data!A2</f>
-        <v>true</v>
-      </c>
-      <c r="C2" s="3" t="str">
-        <f>house_data!A2</f>
-        <v>true</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>8760</v>
       </c>
-      <c r="H2" s="2">
+      <c r="B2" s="2">
         <v>3600</v>
       </c>
-      <c r="I2">
+      <c r="C2">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added working HP on supply side
</commit_message>
<xml_diff>
--- a/GUI.xlsx
+++ b/GUI.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\GitHub\Energy-Balance-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC41FAF-6FB7-485A-B039-6F5B01FC5C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794E1741-9309-4C8D-8D4B-2BE04ABA5368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="storage_data" sheetId="1" r:id="rId1"/>
     <sheet name="pvt_data" sheetId="2" r:id="rId2"/>
     <sheet name="house_data" sheetId="3" r:id="rId3"/>
-    <sheet name="hp_data" sheetId="6" r:id="rId4"/>
-    <sheet name="pv_data" sheetId="7" r:id="rId5"/>
-    <sheet name="weather_data" sheetId="8" r:id="rId6"/>
-    <sheet name="mediator_data" sheetId="4" r:id="rId7"/>
-    <sheet name="simulator_data" sheetId="5" r:id="rId8"/>
+    <sheet name="hp_data" sheetId="4" r:id="rId4"/>
+    <sheet name="pv_data" sheetId="5" r:id="rId5"/>
+    <sheet name="weather_data" sheetId="6" r:id="rId6"/>
+    <sheet name="mediator_data" sheetId="7" r:id="rId7"/>
+    <sheet name="simulator_data" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+  <si>
+    <t>no_of_time_steps</t>
+  </si>
+  <si>
+    <t>time_step</t>
+  </si>
+  <si>
+    <t>repetition_period</t>
+  </si>
   <si>
     <t>storage_is_included</t>
   </si>
@@ -48,24 +57,78 @@
     <t>house_is_included</t>
   </si>
   <si>
+    <t>pv_is_included</t>
+  </si>
+  <si>
+    <t>hp_is_included</t>
+  </si>
+  <si>
     <t>pvt_charges_storage</t>
   </si>
   <si>
+    <t>connection_pv_hp</t>
+  </si>
+  <si>
+    <t>hp_charges_storage</t>
+  </si>
+  <si>
     <t>city</t>
   </si>
   <si>
     <t>house_discharges_storage</t>
   </si>
   <si>
-    <t>no_of_time_steps</t>
-  </si>
-  <si>
-    <t>time_step</t>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
   <si>
     <t>Luzern</t>
   </si>
   <si>
+    <t>solar_latitude</t>
+  </si>
+  <si>
+    <t>cell_efficiency</t>
+  </si>
+  <si>
+    <t>inclination_angle_south</t>
+  </si>
+  <si>
+    <t>inclination_angle_west</t>
+  </si>
+  <si>
+    <t>inclination_angle_east</t>
+  </si>
+  <si>
+    <t>surface_area_horiz</t>
+  </si>
+  <si>
+    <t>surface_area_south</t>
+  </si>
+  <si>
+    <t>surface_area_west</t>
+  </si>
+  <si>
+    <t>surface_area_east</t>
+  </si>
+  <si>
+    <t>collector_temp</t>
+  </si>
+  <si>
+    <t>is_air_source</t>
+  </si>
+  <si>
+    <t>second_law_efficiency</t>
+  </si>
+  <si>
+    <t>max_cop</t>
+  </si>
+  <si>
+    <t>temp_lift</t>
+  </si>
+  <si>
     <t>heating_demand</t>
   </si>
   <si>
@@ -93,33 +156,9 @@
     <t>loss_coeff_2</t>
   </si>
   <si>
-    <t>inclination_angle_south</t>
-  </si>
-  <si>
-    <t>inclination_angle_west</t>
-  </si>
-  <si>
-    <t>inclination_angle_east</t>
-  </si>
-  <si>
-    <t>surface_area_horiz</t>
-  </si>
-  <si>
-    <t>surface_area_south</t>
-  </si>
-  <si>
-    <t>surface_area_west</t>
-  </si>
-  <si>
-    <t>surface_area_east</t>
-  </si>
-  <si>
     <t>max_return_temp</t>
   </si>
   <si>
-    <t>collector_temp</t>
-  </si>
-  <si>
     <t>tank_height</t>
   </si>
   <si>
@@ -153,40 +192,37 @@
     <t>init_charging_temp</t>
   </si>
   <si>
-    <t>repetition_period</t>
-  </si>
-  <si>
-    <t>capacity</t>
-  </si>
-  <si>
-    <t>cell_efficiency</t>
-  </si>
-  <si>
-    <t>second_law_efficiency</t>
-  </si>
-  <si>
-    <t>is_air_source</t>
-  </si>
-  <si>
-    <t>solar_latitude</t>
-  </si>
-  <si>
-    <t>pv_is_included</t>
-  </si>
-  <si>
-    <t>connection_pv_hp</t>
-  </si>
-  <si>
-    <t>hp_charges_storage</t>
-  </si>
-  <si>
-    <t>hp_is_included</t>
-  </si>
-  <si>
-    <t>storage_charging_strategy</t>
-  </si>
-  <si>
-    <t>equally distributed</t>
+    <t>massflow_min</t>
+  </si>
+  <si>
+    <t>massflow_max</t>
+  </si>
+  <si>
+    <t>massflow_air</t>
+  </si>
+  <si>
+    <t>min_approach_temp</t>
+  </si>
+  <si>
+    <t>compressor_duty</t>
+  </si>
+  <si>
+    <t>condenser_duty</t>
+  </si>
+  <si>
+    <t>part_load_efficiency</t>
+  </si>
+  <si>
+    <t>base_cop</t>
+  </si>
+  <si>
+    <t>evaporator_temp_max</t>
+  </si>
+  <si>
+    <t>condenser_temp_max</t>
+  </si>
+  <si>
+    <t>evaporator_temp_min</t>
   </si>
 </sst>
 </file>
@@ -197,7 +233,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +244,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -239,24 +281,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -266,9 +319,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -579,109 +629,109 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>40</v>
+      </c>
+      <c r="C2" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="G2" s="1">
+        <v>95</v>
+      </c>
+      <c r="H2" s="1">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1">
+        <v>4</v>
+      </c>
+      <c r="J2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
         <v>35</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="12"/>
-    </row>
-    <row r="2" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <v>40</v>
-      </c>
-      <c r="C2" s="2">
-        <v>10</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="G2" s="2">
-        <v>95</v>
-      </c>
-      <c r="H2" s="2">
-        <v>20</v>
-      </c>
-      <c r="I2" s="2">
-        <v>10</v>
-      </c>
-      <c r="J2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2">
-        <v>35</v>
-      </c>
-      <c r="L2" s="1"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="1"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -695,105 +745,103 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="A1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="7">
         <v>0.75</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="7">
         <v>3.37</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>1.04E-2</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="13">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>30</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>90</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>30</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>0</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>160</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="1">
         <v>0</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
         <v>0</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="1">
         <v>95</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="1">
         <v>14</v>
       </c>
     </row>
@@ -809,58 +857,58 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>115</v>
+      </c>
+      <c r="B2" s="1">
+        <v>900</v>
+      </c>
+      <c r="C2" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>115</v>
-      </c>
-      <c r="B2" s="2">
-        <v>900</v>
-      </c>
-      <c r="C2" s="2">
-        <v>14</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="D2" s="7">
         <v>0.1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>25</v>
       </c>
-      <c r="F2" s="7">
-        <v>0.16</v>
+      <c r="F2" s="11">
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>
@@ -869,39 +917,127 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61341AFE-9F70-4FA7-8BF0-845A144E344F}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" customWidth="1"/>
+    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>11000</v>
-      </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2">
+    <row r="1" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>12000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="7">
         <v>0.55000000000000004</v>
+      </c>
+      <c r="E2" s="10">
+        <v>6</v>
+      </c>
+      <c r="F2" s="10">
+        <v>4</v>
+      </c>
+      <c r="G2" s="10">
+        <v>45</v>
+      </c>
+      <c r="H2">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="I2">
+        <v>4.1669999999999997E-3</v>
+      </c>
+      <c r="J2">
+        <v>1.63</v>
+      </c>
+      <c r="K2">
+        <v>1.5</v>
+      </c>
+      <c r="L2">
+        <v>0.5</v>
+      </c>
+      <c r="M2">
+        <v>20</v>
+      </c>
+      <c r="N2">
+        <v>-20</v>
+      </c>
+      <c r="O2">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -910,116 +1046,118 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB94CDB9-61E1-4932-B3E2-8E1E2BED6CDC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>26</v>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="7">
         <v>0.23</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>30</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>90</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>30</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>160</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>0</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D84336-4BDD-4290-B4B8-8FB7312C2A0E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="7">
         <v>46.6</v>
       </c>
     </row>
@@ -1029,101 +1167,96 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="19" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="19" style="4" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="19.42578125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="19.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="4"/>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" s="2"/>
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1131,39 +1264,42 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C781A6E-1115-4E08-A78E-093D8B9DB9B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>8760</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>3600</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added heat pump graphs
</commit_message>
<xml_diff>
--- a/GUI.xlsx
+++ b/GUI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\GitHub\Energy-Balance-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA7B8E8-8CC5-4A34-A00C-1257F39EB111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FE5EE4-2595-478B-9312-7E3D46F54C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="storage_data" sheetId="1" r:id="rId1"/>
@@ -628,8 +628,8 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,8 +857,8 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,7 +908,7 @@
         <v>25</v>
       </c>
       <c r="F2" s="11">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated heat pump slides
</commit_message>
<xml_diff>
--- a/GUI.xlsx
+++ b/GUI.xlsx
@@ -1306,4 +1306,290 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E756FDFCB57D0948B915F9BF5E819397" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cef072e22be147cbbcd234eecfd8b59d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9a7d57e2-a6f6-4353-bdc3-995d0b2e54a4" xmlns:ns3="bd5c1ef4-a5a8-4f60-b734-518beb01c7b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a5a5617d388237d6fec17b5909b60a5" ns2:_="" ns3:_="">
+    <xsd:import namespace="9a7d57e2-a6f6-4353-bdc3-995d0b2e54a4"/>
+    <xsd:import namespace="bd5c1ef4-a5a8-4f60-b734-518beb01c7b7"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:Speaker" minOccurs="0"/>
+                <xsd:element ref="ns2:Datum" minOccurs="0"/>
+                <xsd:element ref="ns2:_Flow_SignoffStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9a7d57e2-a6f6-4353-bdc3-995d0b2e54a4" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="10" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="11" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="12" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="16" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="17" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Speaker" ma:index="18" nillable="true" ma:displayName="Speaker" ma:format="Dropdown" ma:list="UserInfo" ma:SharePointGroup="0" ma:internalName="Speaker">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Datum" ma:index="19" nillable="true" ma:displayName="Datum" ma:default="2021-01-02T00:00:00Z" ma:format="DateOnly" ma:internalName="Datum">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_Flow_SignoffStatus" ma:index="20" nillable="true" ma:displayName="Status Unterschrift" ma:internalName="Status_x0020_Unterschrift">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="21" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="22" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="24" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="9a48e02a-304b-44db-a51f-647cba8d1c2e" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="bd5c1ef4-a5a8-4f60-b734-518beb01c7b7" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="13" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="14" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="25" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{8c5dfd34-6cc8-4139-8954-d3e7e36d7eca}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="bd5c1ef4-a5a8-4f60-b734-518beb01c7b7">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A78D058-2DA2-401A-8C8F-821172E7AD68}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2136DE5E-BE9E-4991-BAF0-24002AF3186B}"/>
 </file>
</xml_diff>